<commit_message>
Updating admm solvers and experiment 5
</commit_message>
<xml_diff>
--- a/results/results_5.xlsx
+++ b/results/results_5.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Frobenius Norm Difference" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="247">
   <si>
     <t xml:space="preserve">P1_P3_P4</t>
   </si>
@@ -37,7 +38,7 @@
     <t xml:space="preserve">ADMM</t>
   </si>
   <si>
-    <t xml:space="preserve">ADMM_e</t>
+    <t xml:space="preserve">ADMMe</t>
   </si>
   <si>
     <t xml:space="preserve">m</t>
@@ -79,82 +80,82 @@
     <t xml:space="preserve">12</t>
   </si>
   <si>
-    <t xml:space="preserve">34.06338320795196</t>
-  </si>
-  <si>
-    <t xml:space="preserve">756.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.77030589469091</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47.59581732749939</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.11865711212158</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34.063383207806076</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.770305896873329</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20.008923292160034</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84.58342838287354</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34.06338320754784</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.770305893178804</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21.01443600654602</t>
-  </si>
-  <si>
-    <t xml:space="preserve">92.88760566711426</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34.06338320795059</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.770305894695921</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16.853814363479614</t>
-  </si>
-  <si>
-    <t xml:space="preserve">96.7499647140503</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34.11907324300287</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1250.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.800157162319294</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.3611600399017334</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31.153343200683594</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34.06506737383637</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.769088535940301</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21.6861789226532</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31.154144287109375</t>
+    <t xml:space="preserve">34.02786701679938</t>
+  </si>
+  <si>
+    <t xml:space="preserve">394</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.775270635038462</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45.22190737724304</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.11855697631836</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34.027867016719384</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.775270634926994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.71985363960266</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84.58366680145264</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34.02786701679912</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.775270635059209</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20.666095495224</t>
+  </si>
+  <si>
+    <t xml:space="preserve">92.88842010498047</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34.027867016763736</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.775270634983506</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16.647921085357666</t>
+  </si>
+  <si>
+    <t xml:space="preserve">96.75060749053955</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34.03395086451871</t>
+  </si>
+  <si>
+    <t xml:space="preserve">524</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.7747046264656925</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.97678017616272</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31.16485023498535</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34.02803215168083</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.775594814072104</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56.77750110626221</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31.165613174438477</t>
   </si>
   <si>
     <t xml:space="preserve">60</t>
@@ -166,82 +167,82 @@
     <t xml:space="preserve">15</t>
   </si>
   <si>
-    <t xml:space="preserve">42.942855198124334</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1125.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.83452930733002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">122.14155912399292</t>
-  </si>
-  <si>
-    <t xml:space="preserve">185.76703262329102</t>
-  </si>
-  <si>
-    <t xml:space="preserve">42.942855208965256</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.834529202544172</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37.347102880477905</t>
-  </si>
-  <si>
-    <t xml:space="preserve">193.81296825408936</t>
-  </si>
-  <si>
-    <t xml:space="preserve">42.94285519811878</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.834529307341002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">41.09260702133179</t>
-  </si>
-  <si>
-    <t xml:space="preserve">203.4632911682129</t>
-  </si>
-  <si>
-    <t xml:space="preserve">42.942855198671346</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.834529307903413</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34.40289235115051</t>
-  </si>
-  <si>
-    <t xml:space="preserve">210.86416339874268</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43.01800053534861</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1800.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.846639408233203</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.001248359680176</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75.75345802307129</t>
-  </si>
-  <si>
-    <t xml:space="preserve">42.94482284956436</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.832089344645725</t>
-  </si>
-  <si>
-    <t xml:space="preserve">38.479103326797485</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75.7537899017334</t>
+    <t xml:space="preserve">44.37179262914662</t>
+  </si>
+  <si>
+    <t xml:space="preserve">579</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.927053866314406</t>
+  </si>
+  <si>
+    <t xml:space="preserve">115.27366590499878</t>
+  </si>
+  <si>
+    <t xml:space="preserve">185.76793098449707</t>
+  </si>
+  <si>
+    <t xml:space="preserve">44.37179261459715</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.927053870698028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.29160475730896</t>
+  </si>
+  <si>
+    <t xml:space="preserve">193.8140459060669</t>
+  </si>
+  <si>
+    <t xml:space="preserve">44.37179262916088</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.927053866313557</t>
+  </si>
+  <si>
+    <t xml:space="preserve">41.418724060058594</t>
+  </si>
+  <si>
+    <t xml:space="preserve">203.46449661254883</t>
+  </si>
+  <si>
+    <t xml:space="preserve">44.37179262916894</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.927053866524837</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33.57557272911072</t>
+  </si>
+  <si>
+    <t xml:space="preserve">210.8655481338501</t>
+  </si>
+  <si>
+    <t xml:space="preserve">44.379918835663176</t>
+  </si>
+  <si>
+    <t xml:space="preserve">761</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.932106778798337</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.105797052383423</t>
+  </si>
+  <si>
+    <t xml:space="preserve">75.77054023742676</t>
+  </si>
+  <si>
+    <t xml:space="preserve">44.37199445225531</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.927070665286104</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100.10611772537231</t>
+  </si>
+  <si>
+    <t xml:space="preserve">75.77112579345703</t>
   </si>
   <si>
     <t xml:space="preserve">70</t>
@@ -253,82 +254,85 @@
     <t xml:space="preserve">17</t>
   </si>
   <si>
-    <t xml:space="preserve">49.52464433520109</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1496.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.434123508019802</t>
-  </si>
-  <si>
-    <t xml:space="preserve">244.44855165481567</t>
-  </si>
-  <si>
-    <t xml:space="preserve">353.4545192718506</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49.524644335229624</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.434123507609181</t>
-  </si>
-  <si>
-    <t xml:space="preserve">65.08190774917603</t>
-  </si>
-  <si>
-    <t xml:space="preserve">351.8171796798706</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49.52464434105078</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.43412350902586</t>
-  </si>
-  <si>
-    <t xml:space="preserve">79.30377769470215</t>
-  </si>
-  <si>
-    <t xml:space="preserve">376.617130279541</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49.52464433521877</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.434123507849254</t>
-  </si>
-  <si>
-    <t xml:space="preserve">64.32510685920715</t>
-  </si>
-  <si>
-    <t xml:space="preserve">385.4498338699341</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49.63787587629511</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2450.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.461398514810476</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.092178583145142</t>
-  </si>
-  <si>
-    <t xml:space="preserve">136.4016284942627</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49.5269106807427</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.435279944475138</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50.046464681625366</t>
-  </si>
-  <si>
-    <t xml:space="preserve">136.4023380279541</t>
+    <t xml:space="preserve">49.534232602202216</t>
+  </si>
+  <si>
+    <t xml:space="preserve">764</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.514387396439108</t>
+  </si>
+  <si>
+    <t xml:space="preserve">240.64546179771423</t>
+  </si>
+  <si>
+    <t xml:space="preserve">353.4559602737427</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49.534232602040525</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.514387396472342</t>
+  </si>
+  <si>
+    <t xml:space="preserve">63.72751212120056</t>
+  </si>
+  <si>
+    <t xml:space="preserve">351.8188533782959</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49.534232602189064</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.514387396374365</t>
+  </si>
+  <si>
+    <t xml:space="preserve">76.93835616111755</t>
+  </si>
+  <si>
+    <t xml:space="preserve">376.6189308166504</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49.53423260218911</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.514387396589</t>
+  </si>
+  <si>
+    <t xml:space="preserve">63.129408836364746</t>
+  </si>
+  <si>
+    <t xml:space="preserve">385.451771736145</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49.54585131644184</t>
+  </si>
+  <si>
+    <t xml:space="preserve">985</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.513907431240833</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17.782227277755737</t>
+  </si>
+  <si>
+    <t xml:space="preserve">136.4245729446411</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49.53446325258054</t>
+  </si>
+  <si>
+    <t xml:space="preserve">763</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.514508576781283</t>
+  </si>
+  <si>
+    <t xml:space="preserve">147.69799399375916</t>
+  </si>
+  <si>
+    <t xml:space="preserve">136.4252004623413</t>
   </si>
   <si>
     <t xml:space="preserve">80</t>
@@ -340,82 +344,85 @@
     <t xml:space="preserve">20</t>
   </si>
   <si>
-    <t xml:space="preserve">58.48054339424981</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2000.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.33836560016486</t>
-  </si>
-  <si>
-    <t xml:space="preserve">504.33039021492004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">592.7852668762207</t>
-  </si>
-  <si>
-    <t xml:space="preserve">58.48054339428724</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.338365600282662</t>
-  </si>
-  <si>
-    <t xml:space="preserve">107.84147334098816</t>
-  </si>
-  <si>
-    <t xml:space="preserve">591.5593662261963</t>
-  </si>
-  <si>
-    <t xml:space="preserve">58.48054339429539</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.33836560043101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">140.36559581756592</t>
-  </si>
-  <si>
-    <t xml:space="preserve">621.8010663986206</t>
-  </si>
-  <si>
-    <t xml:space="preserve">58.480543394303226</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.338365600437498</t>
-  </si>
-  <si>
-    <t xml:space="preserve">113.54236888885498</t>
-  </si>
-  <si>
-    <t xml:space="preserve">630.4594774246216</t>
-  </si>
-  <si>
-    <t xml:space="preserve">58.60756284173028</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3200.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.363384901162096</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.786485433578491</t>
-  </si>
-  <si>
-    <t xml:space="preserve">215.57808113098145</t>
-  </si>
-  <si>
-    <t xml:space="preserve">58.48308268797272</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.337823785765737</t>
-  </si>
-  <si>
-    <t xml:space="preserve">65.45083451271057</t>
-  </si>
-  <si>
-    <t xml:space="preserve">215.57884407043457</t>
+    <t xml:space="preserve">58.63807788866084</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.479258004326432</t>
+  </si>
+  <si>
+    <t xml:space="preserve">513.1670289039612</t>
+  </si>
+  <si>
+    <t xml:space="preserve">592.7872867584229</t>
+  </si>
+  <si>
+    <t xml:space="preserve">58.63807788865451</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.479258004257355</t>
+  </si>
+  <si>
+    <t xml:space="preserve">104.94539070129395</t>
+  </si>
+  <si>
+    <t xml:space="preserve">591.5616025924683</t>
+  </si>
+  <si>
+    <t xml:space="preserve">58.638077888678055</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.47925800431862</t>
+  </si>
+  <si>
+    <t xml:space="preserve">139.34290742874146</t>
+  </si>
+  <si>
+    <t xml:space="preserve">621.8035354614258</t>
+  </si>
+  <si>
+    <t xml:space="preserve">58.638077888650905</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.479258004508994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">113.09853935241699</t>
+  </si>
+  <si>
+    <t xml:space="preserve">630.4620723724365</t>
+  </si>
+  <si>
+    <t xml:space="preserve">58.652031884103245</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1271</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.483669355201814</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.033101558685303</t>
+  </si>
+  <si>
+    <t xml:space="preserve">215.60846614837646</t>
+  </si>
+  <si>
+    <t xml:space="preserve">58.63833497773061</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.478673419576326</t>
+  </si>
+  <si>
+    <t xml:space="preserve">297.2330231666565</t>
+  </si>
+  <si>
+    <t xml:space="preserve">215.60913753509521</t>
   </si>
   <si>
     <t xml:space="preserve">90</t>
@@ -427,163 +434,334 @@
     <t xml:space="preserve">22</t>
   </si>
   <si>
-    <t xml:space="preserve">64.48106546414428</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2486.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.808409200940346</t>
-  </si>
-  <si>
-    <t xml:space="preserve">906.7193207740784</t>
-  </si>
-  <si>
-    <t xml:space="preserve">934.9482765197754</t>
-  </si>
-  <si>
-    <t xml:space="preserve">64.48106546668984</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.808409213629025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">169.14387321472168</t>
-  </si>
-  <si>
-    <t xml:space="preserve">929.0716257095337</t>
-  </si>
-  <si>
-    <t xml:space="preserve">64.48106546409852</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.808409200975705</t>
-  </si>
-  <si>
-    <t xml:space="preserve">242.77166152000427</t>
-  </si>
-  <si>
-    <t xml:space="preserve">970.2338275909424</t>
-  </si>
-  <si>
-    <t xml:space="preserve">64.48106546432632</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.808409200679678</t>
-  </si>
-  <si>
-    <t xml:space="preserve">188.69962358474731</t>
-  </si>
-  <si>
-    <t xml:space="preserve">972.6177473068237</t>
-  </si>
-  <si>
-    <t xml:space="preserve">64.64741700663556</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4050.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.818214415041513</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.839452266693115</t>
-  </si>
-  <si>
-    <t xml:space="preserve">315.7778625488281</t>
-  </si>
-  <si>
-    <t xml:space="preserve">64.48395846825234</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.80762138023288</t>
-  </si>
-  <si>
-    <t xml:space="preserve">112.40577030181885</t>
-  </si>
-  <si>
-    <t xml:space="preserve">315.77819442749023</t>
+    <t xml:space="preserve">63.42093152535007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1273</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.709921709103636</t>
+  </si>
+  <si>
+    <t xml:space="preserve">872.4289844036102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">934.9512577056885</t>
+  </si>
+  <si>
+    <t xml:space="preserve">63.420931525306315</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.709921709024188</t>
+  </si>
+  <si>
+    <t xml:space="preserve">165.1228425502777</t>
+  </si>
+  <si>
+    <t xml:space="preserve">929.0747365951538</t>
+  </si>
+  <si>
+    <t xml:space="preserve">63.42093152534592</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.7099217090216</t>
+  </si>
+  <si>
+    <t xml:space="preserve">230.26661944389343</t>
+  </si>
+  <si>
+    <t xml:space="preserve">970.237117767334</t>
+  </si>
+  <si>
+    <t xml:space="preserve">63.420931525239126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.709921712629146</t>
+  </si>
+  <si>
+    <t xml:space="preserve">190.2739245891571</t>
+  </si>
+  <si>
+    <t xml:space="preserve">972.6211738586426</t>
+  </si>
+  <si>
+    <t xml:space="preserve">63.43934751785906</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1602</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.714775180491019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32.51755952835083</t>
+  </si>
+  <si>
+    <t xml:space="preserve">315.8161287307739</t>
+  </si>
+  <si>
+    <t xml:space="preserve">63.421224980840236</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.7106522893599</t>
+  </si>
+  <si>
+    <t xml:space="preserve">377.15524196624756</t>
+  </si>
+  <si>
+    <t xml:space="preserve">315.8168001174927</t>
   </si>
   <si>
     <t xml:space="preserve">100</t>
   </si>
   <si>
-    <t xml:space="preserve">75.08882784592046</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3125.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11.787032337126119</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1816.7961864471436</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1393.461519241333</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75.0888278527188</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11.787032338799346</t>
-  </si>
-  <si>
-    <t xml:space="preserve">273.2134244441986</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1381.3975591659546</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75.0888278445673</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11.787032329609486</t>
-  </si>
-  <si>
-    <t xml:space="preserve">541.9641969203949</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1434.9829711914062</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75.0888278462653</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11.787032335290679</t>
-  </si>
-  <si>
-    <t xml:space="preserve">295.50924158096313</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1438.5871601104736</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75.28975580055071</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5000.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11.805381093394429</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.435949563980103</t>
-  </si>
-  <si>
-    <t xml:space="preserve">439.46918392181396</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75.09200333481814</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11.788338746019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">120.97706532478333</t>
-  </si>
-  <si>
-    <t xml:space="preserve">439.46989345550537</t>
+    <t xml:space="preserve">73.19948703613925</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1566</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.625264888222711</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1770.3322179317474</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1393.465012550354</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73.1994870418414</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.625264899395281</t>
+  </si>
+  <si>
+    <t xml:space="preserve">275.46490693092346</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1381.4013385772705</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73.1994870361353</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.625264887829259</t>
+  </si>
+  <si>
+    <t xml:space="preserve">453.7300350666046</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1434.9867582321167</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73.19948703609045</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.62526488837578</t>
+  </si>
+  <si>
+    <t xml:space="preserve">300.23713779449463</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1438.5908241271973</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73.22178831363972</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2052</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.633212553752047</t>
+  </si>
+  <si>
+    <t xml:space="preserve">46.43649935722351</t>
+  </si>
+  <si>
+    <t xml:space="preserve">439.5158586502075</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73.19981571932892</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1563</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.62493853301096</t>
+  </si>
+  <si>
+    <t xml:space="preserve">532.7208988666534</t>
+  </si>
+  <si>
+    <t xml:space="preserve">439.51640129089355</t>
+  </si>
+  <si>
+    <t xml:space="preserve">||P1_P3_P4 - admm||_F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">||P1_P3_P4 - admme||_F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">||PLS_P4 - admm||_F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">||PLS_P4 - admme||_F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">||PMN_P3 - admm||_F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">||PMN_P3 - admme||_F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">||PMX - admm||_F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">||PMX - admme||_F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.02405366088765324</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0020928074643539307</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.024053660319974392</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0020928077889786813</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.024053660786209147</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.002092807275753626</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.02405366095308631</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.002092807685216926</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.013942463095975136</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0011630994674067213</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.01394245134695597</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.001163084442924733</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.013942463125009751</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0011630995098158743</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.013942462187119503</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0011630990431050754</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.024292515541976187</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0017404451545448229</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.024292515475316693</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.001740444521334036</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.024292515588288162</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.001740445417196322</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.02429251528910697</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.001740444602567471</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.039375317807319954</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0036227606445651665</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.03937531756641347</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0036227610650156005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.03937531777634481</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.003622760619972328</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.03937531771563106</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0036227615903160876</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.03964413871028897</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.004103105041516115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.03964413838392501</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.004103105350397715</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.039644138416880186</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.004103105310327483</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.03964414337364699</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.004103092464904088</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.034315188380373236</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0047074308736956855</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.034315372804033455</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00470770371668914</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.03431518783819006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.004707429303049393</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.03431518845198002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.004707430617473698</t>
   </si>
 </sst>
 </file>
@@ -644,19 +822,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEC9BA4"/>
+        <fgColor rgb="FFFFA6A6"/>
         <bgColor rgb="FFFFAA95"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFAA95"/>
-        <bgColor rgb="FFEC9BA4"/>
+        <bgColor rgb="FFFFA6A6"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFE994"/>
+        <fgColor rgb="FFFFFFA6"/>
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
@@ -805,9 +983,9 @@
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFE994"/>
+      <rgbColor rgb="FFFFFFA6"/>
       <rgbColor rgb="FFAFD095"/>
-      <rgbColor rgb="FFEC9BA4"/>
+      <rgbColor rgb="FFFFA6A6"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFAA95"/>
       <rgbColor rgb="FF3366FF"/>
@@ -1029,7 +1207,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="10.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="21.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="19.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="21.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="21.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="10.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="21.32"/>
@@ -1039,12 +1217,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="10.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="21.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="19.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="21.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="21.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="10.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="21.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="19.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="21.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="21.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="10.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="21.32"/>
@@ -1366,7 +1544,7 @@
         <v>41</v>
       </c>
       <c r="AO3" s="0" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="AP3" s="0" t="s">
         <v>42</v>
@@ -1503,7 +1681,7 @@
         <v>70</v>
       </c>
       <c r="AO4" s="0" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="AP4" s="0" t="s">
         <v>71</v>
@@ -1640,298 +1818,298 @@
         <v>99</v>
       </c>
       <c r="AO5" s="0" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="AP5" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AQ5" s="0" t="s">
         <v>75</v>
       </c>
       <c r="AR5" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AS5" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C6" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>104</v>
-      </c>
       <c r="E6" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G6" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="M6" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="H6" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="K6" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="L6" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="M6" s="0" t="s">
-        <v>107</v>
-      </c>
       <c r="N6" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="P6" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="Q6" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="R6" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="S6" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="T6" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="U6" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="V6" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="W6" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="X6" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="Y6" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="Z6" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AA6" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AB6" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AC6" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AD6" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AE6" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="AF6" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AG6" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AH6" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AI6" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AJ6" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AK6" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AL6" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AM6" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AN6" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AO6" s="0" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="AP6" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AQ6" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AR6" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AS6" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E7" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="H7" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="F7" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>133</v>
-      </c>
       <c r="I7" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="M7" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="J7" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="K7" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="L7" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="M7" s="0" t="s">
-        <v>136</v>
-      </c>
       <c r="N7" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="O7" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="P7" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="Q7" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="R7" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="S7" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="T7" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="U7" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="V7" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="W7" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="X7" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="Y7" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="Z7" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="AA7" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AB7" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="AC7" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="AD7" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AE7" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="AF7" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="AG7" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AH7" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="AI7" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="AJ7" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="AK7" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="AL7" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="AM7" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="AN7" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="AO7" s="0" t="s">
-        <v>153</v>
+        <v>125</v>
       </c>
       <c r="AP7" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="AQ7" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="AR7" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="AS7" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>16</v>
@@ -1943,127 +2121,406 @@
         <v>16</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="H8" s="0" t="s">
         <v>16</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="K8" s="0" t="s">
         <v>16</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="N8" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="O8" s="0" t="s">
         <v>16</v>
       </c>
       <c r="P8" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="Q8" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="R8" s="0" t="s">
         <v>16</v>
       </c>
       <c r="S8" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="T8" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="U8" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="V8" s="0" t="s">
         <v>16</v>
       </c>
       <c r="W8" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="X8" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="Y8" s="0" t="s">
         <v>16</v>
       </c>
       <c r="Z8" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="AA8" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="AB8" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="AC8" s="0" t="s">
         <v>16</v>
       </c>
       <c r="AD8" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="AE8" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="AF8" s="0" t="s">
         <v>16</v>
       </c>
       <c r="AG8" s="0" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="AH8" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="AI8" s="0" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="AJ8" s="0" t="s">
         <v>16</v>
       </c>
       <c r="AK8" s="0" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="AL8" s="0" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="AM8" s="0" t="s">
         <v>16</v>
       </c>
       <c r="AN8" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="AO8" s="0" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="AP8" s="0" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="AQ8" s="0" t="s">
         <v>16</v>
       </c>
       <c r="AR8" s="0" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="AS8" s="0" t="s">
-        <v>187</v>
+        <v>190</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="24.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="24.39"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>